<commit_message>
Fixed issue where driver changes PWM control file location. Added text file config of outputs. Added PCA9685 code. Fixed bug in LSM303DLHC code.
</commit_message>
<xml_diff>
--- a/Beaglebone Pinmux Worksheet.xlsx
+++ b/Beaglebone Pinmux Worksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24465" windowHeight="6360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25320" windowHeight="9765"/>
   </bookViews>
   <sheets>
     <sheet name="Pinmux" sheetId="1" r:id="rId1"/>
@@ -1182,7 +1182,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,6 +2428,10 @@
       </c>
       <c r="F47" t="s">
         <v>216</v>
+      </c>
+      <c r="G47">
+        <f>32*3+19</f>
+        <v>115</v>
       </c>
       <c r="M47" t="s">
         <v>221</v>

</xml_diff>